<commit_message>
reorganize the test suite
</commit_message>
<xml_diff>
--- a/Aspire test suites v.1.0.xlsx
+++ b/Aspire test suites v.1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pcha/Documents/WorkSP/AspireAppDemo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1CBBE06-50E8-4740-BBA3-1A0DB9BD1869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0103149E-EBA6-854D-88E0-08FEB419921B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="800" yWindow="500" windowWidth="35000" windowHeight="21900" tabRatio="853" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2303,7 +2303,7 @@
     <xf numFmtId="0" fontId="43" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="176">
+  <cellXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2744,6 +2744,9 @@
     </xf>
     <xf numFmtId="0" fontId="47" fillId="9" borderId="5" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="48" fillId="9" borderId="5" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="42" fillId="9" borderId="5" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="20% - Accent1 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -7866,7 +7869,7 @@
   <dimension ref="A3:H60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.33203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -7888,11 +7891,11 @@
       <c r="H3" s="122"/>
     </row>
     <row r="5" spans="1:8" ht="26" x14ac:dyDescent="0.15">
-      <c r="B5" s="114" t="s">
+      <c r="C5" s="176" t="s">
         <v>312</v>
       </c>
-      <c r="D5" s="114"/>
-      <c r="E5" s="114"/>
+      <c r="D5" s="176"/>
+      <c r="E5" s="176"/>
       <c r="F5" s="114"/>
     </row>
     <row r="9" spans="1:8" ht="15.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -8106,7 +8109,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="C5:E5"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="B9:B10"/>
@@ -9383,9 +9387,9 @@
   </sheetPr>
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11347,9 +11351,9 @@
   </sheetPr>
   <dimension ref="A1:P461"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>